<commit_message>
Correct labels to full names
</commit_message>
<xml_diff>
--- a/prelim_results/summary_stats.xlsx
+++ b/prelim_results/summary_stats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="214">
   <si>
     <t>Assembly</t>
   </si>
@@ -632,15 +632,6 @@
     <t>M36606</t>
   </si>
   <si>
-    <t>Meta</t>
-  </si>
-  <si>
-    <t>Spades</t>
-  </si>
-  <si>
-    <t>Abyss</t>
-  </si>
-  <si>
     <t>Velvet</t>
   </si>
   <si>
@@ -669,6 +660,15 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>Metassembler</t>
+  </si>
+  <si>
+    <t>SPAdes</t>
+  </si>
+  <si>
+    <t>ABySS</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1380,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Meta</c:v>
+                  <c:v>Metassembler</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1639,7 +1639,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Spades</c:v>
+                  <c:v>SPAdes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1770,7 +1770,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>2.516922097039828</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.05661198488279</c:v>
@@ -1891,7 +1891,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Abyss</c:v>
+                  <c:v>ABySS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2406,11 +2406,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2138156768"/>
-        <c:axId val="-2138119040"/>
+        <c:axId val="2126543776"/>
+        <c:axId val="2127929888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2138156768"/>
+        <c:axId val="2126543776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2420,7 +2420,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138119040"/>
+        <c:crossAx val="2127929888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2428,7 +2428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138119040"/>
+        <c:axId val="2127929888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2439,7 +2439,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2138156768"/>
+        <c:crossAx val="2126543776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2514,7 +2514,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Meta</c:v>
+                  <c:v>Metassembler</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2773,7 +2773,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Spades</c:v>
+                  <c:v>SPAdes</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3025,7 +3025,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Abyss</c:v>
+                  <c:v>ABySS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3540,11 +3540,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2099447808"/>
-        <c:axId val="-2098312720"/>
+        <c:axId val="2126521600"/>
+        <c:axId val="2126518432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2099447808"/>
+        <c:axId val="2126521600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3554,7 +3554,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2098312720"/>
+        <c:crossAx val="2126518432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3562,7 +3562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2098312720"/>
+        <c:axId val="2126518432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3573,7 +3573,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2099447808"/>
+        <c:crossAx val="2126521600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -16202,8 +16202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AK159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U44" sqref="U44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16315,12 +16315,12 @@
         <v>200</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="B3">
         <v>4.5602049238149709</v>
@@ -16433,10 +16433,10 @@
     </row>
     <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>202</v>
-      </c>
-      <c r="B4">
-        <v>2.5169220970398278</v>
+        <v>212</v>
+      </c>
+      <c r="B4" t="s">
+        <v>213</v>
       </c>
       <c r="C4">
         <v>2.0566119848827902</v>
@@ -16546,7 +16546,7 @@
     </row>
     <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B5">
         <v>4.5285752985395558</v>
@@ -16659,7 +16659,7 @@
     </row>
     <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B6">
         <v>3.5704106894712209</v>
@@ -16877,12 +16877,12 @@
         <v>200</v>
       </c>
       <c r="AK8" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
       <c r="B9">
         <v>10.208142605239807</v>
@@ -16995,7 +16995,7 @@
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
       <c r="B10">
         <v>9.1049805682822598</v>
@@ -17108,7 +17108,7 @@
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="B11">
         <v>10.499750144695106</v>
@@ -17221,7 +17221,7 @@
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B12">
         <v>9.9782470078902303</v>
@@ -17334,7 +17334,7 @@
     </row>
     <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:37" x14ac:dyDescent="0.2">
@@ -19920,16 +19920,16 @@
         <v>5.48</v>
       </c>
       <c r="T1" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>210</v>
       </c>
       <c r="X1" s="5" t="s">
         <v>161</v>
@@ -19938,10 +19938,10 @@
         <v>163</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="16" x14ac:dyDescent="0.25">
@@ -22781,7 +22781,7 @@
         <v>0</v>
       </c>
       <c r="T37" s="11" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="U37" s="7">
         <v>100.89016555400654</v>

</xml_diff>

<commit_message>
Move to clustered bars
</commit_message>
<xml_diff>
--- a/prelim_results/summary_stats.xlsx
+++ b/prelim_results/summary_stats.xlsx
@@ -1339,21 +1339,28 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0"/>
@@ -1364,12 +1371,37 @@
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1386,15 +1418,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'score plots'!$B$2:$AK$2</c:f>
@@ -1628,263 +1660,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'score plots'!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SPAdes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'score plots'!$B$2:$AK$2</c:f>
-              <c:strCache>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>M05964</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>M07572</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>M10540</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>M16180</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>M26026</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>M26032</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>M27986</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>M27987</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>M28356</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>M28405</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>M28687</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>M28702</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>M28745</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>M28770</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>M28801</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>M28853</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>M28888</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>M29179</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>M29197</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>M29202</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>M29227</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>M29307</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>M29323</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>M29331</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>M29400</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>M29658</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>M29684</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>M29695</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>M29697</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>M36557</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>M36564</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>M36580</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>M36582</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>M36605</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>M36606</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>M37982</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'score plots'!$B$4:$AK$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.05661198488279</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.840822252376486</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.67794291693401</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.867827150671271</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.18580866680459</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.075327289993257</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.889353214363893</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.923581670663164</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.54287528868442</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.840236565472189</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.230105174961993</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>4.255109470325407</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.663484304781248</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.649165123777619</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.320402180951771</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.146356339935678</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.242040537946765</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.722696064221506</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>1.44610002145936</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>1.424549291151602</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.674080368457981</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.710980485268073</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.650590379516077</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.695109889674635</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.953756744115955</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4.278176549493327</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.529872931536401</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>4.05256547235284</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>4.110418891146172</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.954077694656749</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.910150915054812</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>2.808489393166015</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.104669397665173</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.271454893511381</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3.953717672596417</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'score plots'!$A$5</c:f>
@@ -1897,19 +1676,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
             <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="63000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'score plots'!$B$2:$AK$2</c:f>
@@ -2143,11 +1918,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'score plots'!$A$6</c:f>
@@ -2159,9 +1933,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'score plots'!$B$2:$AK$2</c:f>
@@ -2395,7 +2176,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2405,22 +2185,54 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="2126543776"/>
-        <c:axId val="2127929888"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2129249328"/>
+        <c:axId val="-2129252688"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="2126543776"/>
+        <c:axId val="-2129249328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127929888"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:tint val="75000"/>
+                <a:shade val="95000"/>
+                <a:satMod val="105000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2129252688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2428,36 +2240,138 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127929888"/>
+        <c:axId val="-2129252688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:tint val="75000"/>
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126543776"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:tint val="75000"/>
+                <a:shade val="95000"/>
+                <a:satMod val="105000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2129249328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:tint val="75000"/>
+          <a:shade val="95000"/>
+          <a:satMod val="105000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -2473,21 +2387,28 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="101"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="1"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
-          <a:bodyPr/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" sz="1400" b="0"/>
@@ -2498,12 +2419,37 @@
       </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2520,15 +2466,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
             <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'score plots'!$B$8:$AK$8</c:f>
@@ -2762,263 +2708,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'score plots'!$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>SPAdes</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'score plots'!$B$8:$AK$8</c:f>
-              <c:strCache>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>M05964</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>M07572</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>M10540</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>M16180</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>M26026</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>M26032</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>M27986</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>M27987</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>M28356</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>M28405</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>M28687</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>M28702</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>M28745</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>M28770</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>M28801</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>M28853</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>M28888</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>M29179</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>M29197</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>M29202</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>M29227</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>M29307</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>M29323</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>M29331</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>M29400</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>M29658</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>M29684</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>M29695</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>M29697</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>M36557</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>M36564</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>M36580</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>M36582</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>M36605</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>M36606</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Score</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'score plots'!$B$10:$AK$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>9.10498056828226</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.93348265077278</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.782709760978262</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.87609655062103</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.852341059256834</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10.47681002798123</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.12409116609385</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.993033083454795</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10.41448781530303</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.81813382695331</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>9.95688853839464</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9.552464373429655</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10.13503660277564</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>9.747802058456736</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>10.1500088753377</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9.758905342029431</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9.74248071803874</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>10.10582224327318</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>8.856400213316557</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>8.690846201842083</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>8.698845074835734</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.82584772568286</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>11.1053675817834</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.714473885959887</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>10.02388270230337</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>10.1340510737686</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>10.2750844134717</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>9.732448017275377</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>10.27042056346032</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>10.01192402497565</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>10.10566752682227</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9.112567590654368</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9.347637195827472</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9.60080838275986</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>7.738244582607907</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>10.20899831472631</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>'score plots'!$A$11</c:f>
@@ -3031,19 +2724,15 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
             <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                  <a:alpha val="63000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
+            <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'score plots'!$B$8:$AK$8</c:f>
@@ -3277,11 +2966,10 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>'score plots'!$A$12</c:f>
@@ -3293,9 +2981,16 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'score plots'!$B$8:$AK$8</c:f>
@@ -3529,7 +3224,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3539,22 +3233,54 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="2126521600"/>
-        <c:axId val="2126518432"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2121576480"/>
+        <c:axId val="-2121671280"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="2126521600"/>
+        <c:axId val="-2121576480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126518432"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:tint val="75000"/>
+                <a:shade val="95000"/>
+                <a:satMod val="105000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2121671280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3562,36 +3288,138 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126518432"/>
+        <c:axId val="-2121671280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:tint val="75000"/>
+                  <a:shade val="95000"/>
+                  <a:satMod val="105000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126521600"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:tint val="75000"/>
+                <a:shade val="95000"/>
+                <a:satMod val="105000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="solid"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2121576480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
+        <a:effectLst/>
       </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:tint val="75000"/>
+          <a:shade val="95000"/>
+          <a:satMod val="105000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:prstDash val="solid"/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -3600,20 +3428,980 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="101">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:lineWidthScale>3</cs:lineWidthScale>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="dk1">
+        <a:tint val="85000"/>
+      </a:schemeClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="dk1">
+        <a:tint val="25000"/>
+      </a:schemeClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="101">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:lineWidthScale>3</cs:lineWidthScale>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="dk1">
+        <a:tint val="85000"/>
+      </a:schemeClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="bg1"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln cap="rnd">
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <a:schemeClr val="dk1">
+        <a:tint val="25000"/>
+      </a:schemeClr>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="1">
+      <a:schemeClr val="tx1">
+        <a:tint val="75000"/>
+      </a:schemeClr>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
+      <xdr:colOff>25400</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:rowOff>106362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>515937</xdr:colOff>
+      <xdr:colOff>477837</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16202,8 +16990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AK159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:A12"/>
+    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>